<commit_message>
atualizaçoes do dia 25/05
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\veteranoFC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FD8CD9-DC5F-453B-BEE5-8ECFF1FBC831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B71B16-9598-4815-AF05-4A58CDE8DA53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="10455" windowHeight="10905" xr2:uid="{FCB38D75-D398-4970-9FB8-9D07E6F74D50}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{FCB38D75-D398-4970-9FB8-9D07E6F74D50}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="49">
   <si>
     <t>artilharia</t>
   </si>
@@ -163,6 +163,15 @@
   </si>
   <si>
     <t>Ildo</t>
+  </si>
+  <si>
+    <t>Chulepe</t>
+  </si>
+  <si>
+    <t>Dinho</t>
+  </si>
+  <si>
+    <t>Vagner</t>
   </si>
 </sst>
 </file>
@@ -178,12 +187,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFDCBC3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -198,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -210,12 +231,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFDCBC3"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -524,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6074CA3F-4164-45B5-860A-DF8F6E2E9DBD}">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,7 +568,7 @@
     <col min="11" max="11" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -551,7 +579,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -561,14 +589,14 @@
       <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -576,19 +604,23 @@
         <v>26</v>
       </c>
       <c r="C3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C4">
-        <v>5</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="6"/>
       <c r="G4" t="s">
         <v>10</v>
       </c>
@@ -610,31 +642,44 @@
       <c r="M4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C5">
-        <v>4</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6"/>
       <c r="G5" s="1">
         <v>45725</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O5" t="s">
+        <v>19</v>
+      </c>
+      <c r="P5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>4</v>
       </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6"/>
       <c r="G6" t="s">
         <v>13</v>
       </c>
@@ -656,8 +701,14 @@
       <c r="M6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O6" t="s">
+        <v>34</v>
+      </c>
+      <c r="P6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -665,13 +716,15 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>3</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6"/>
       <c r="G7" s="1">
         <v>45732</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -681,6 +734,8 @@
       <c r="C8">
         <v>3</v>
       </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6"/>
       <c r="G8" t="s">
         <v>19</v>
       </c>
@@ -702,8 +757,14 @@
       <c r="M8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O8" t="s">
+        <v>35</v>
+      </c>
+      <c r="P8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -713,20 +774,24 @@
       <c r="C9">
         <v>3</v>
       </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6"/>
       <c r="G9" s="1">
         <v>45739</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C10">
-        <v>2</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
       <c r="G10" t="s">
         <v>13</v>
       </c>
@@ -749,33 +814,36 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="6"/>
       <c r="G11" s="1">
         <v>45746</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="6"/>
       <c r="G12" t="s">
         <v>13</v>
       </c>
@@ -798,30 +866,34 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="6"/>
       <c r="G13" s="1">
         <v>45760</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C14">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="6"/>
       <c r="G14" t="s">
         <v>13</v>
       </c>
@@ -844,30 +916,34 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="C15">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="6"/>
       <c r="G15" s="1">
         <v>45767</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6"/>
       <c r="G16" t="s">
         <v>13</v>
       </c>
@@ -895,11 +971,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
+      <c r="D17" s="5"/>
+      <c r="E17" s="6"/>
       <c r="G17" s="1">
         <v>45781</v>
       </c>
@@ -908,6 +986,14 @@
       <c r="A18">
         <v>16</v>
       </c>
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="6"/>
       <c r="G18" t="s">
         <v>13</v>
       </c>
@@ -925,17 +1011,33 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="6"/>
       <c r="G19" s="1">
         <v>45795</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
       <c r="B20" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="6"/>
       <c r="G20" t="s">
         <v>13</v>
       </c>
@@ -959,79 +1061,163 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
       <c r="B21" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
+        <v>48</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="6"/>
+      <c r="G21" s="1">
+        <v>45802</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>42</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="6"/>
+      <c r="G22" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" t="s">
+        <v>24</v>
+      </c>
+      <c r="I22" s="4">
+        <v>5</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K22" s="3">
+        <v>4</v>
+      </c>
+      <c r="L22" t="s">
+        <v>21</v>
+      </c>
+      <c r="M22" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="G23" t="s">
-        <v>33</v>
-      </c>
+      <c r="D23" s="5"/>
+      <c r="E23" s="6"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="G24" t="s">
-        <v>19</v>
-      </c>
-      <c r="H24">
-        <v>4</v>
-      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="6"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="G25" t="s">
-        <v>34</v>
-      </c>
-      <c r="H25">
-        <v>3</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="D25" s="5">
+        <v>2</v>
+      </c>
+      <c r="E25" s="6"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="5">
+        <v>1</v>
+      </c>
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="5">
+        <v>1</v>
+      </c>
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="5">
+        <v>1</v>
+      </c>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29" s="5">
+        <v>1</v>
+      </c>
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="5">
+        <v>1</v>
+      </c>
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>41</v>
       </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G27" t="s">
-        <v>35</v>
-      </c>
-      <c r="H27">
-        <v>1</v>
-      </c>
+      <c r="D31" s="5">
+        <v>1</v>
+      </c>
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="5">
+        <v>1</v>
+      </c>
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="5">
+        <v>1</v>
+      </c>
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="5">
+        <v>1</v>
+      </c>
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D35" s="5">
+        <v>1</v>
+      </c>
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D36" s="5"/>
+      <c r="E36" s="6"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B20:B26">
-    <sortCondition ref="B20:B26"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:C21">
+    <sortCondition descending="1" ref="C3:C21"/>
   </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Dados corrigidos do dia 25/05 e página resultado com acordeon
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\veteranoFC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B71B16-9598-4815-AF05-4A58CDE8DA53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6642DD77-43E0-487B-A296-7D648FB2AEF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{FCB38D75-D398-4970-9FB8-9D07E6F74D50}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="49">
   <si>
     <t>artilharia</t>
   </si>
@@ -153,9 +153,6 @@
     <t>Thiago</t>
   </si>
   <si>
-    <t>Beleno</t>
-  </si>
-  <si>
     <t>Adriano</t>
   </si>
   <si>
@@ -172,6 +169,9 @@
   </si>
   <si>
     <t>Vagner</t>
+  </si>
+  <si>
+    <t>Belone</t>
   </si>
 </sst>
 </file>
@@ -554,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6074CA3F-4164-45B5-860A-DF8F6E2E9DBD}">
   <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,7 +921,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -1031,7 +1031,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1065,7 +1065,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1114,7 +1114,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D25" s="5">
         <v>2</v>
@@ -1132,7 +1132,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D27" s="5">
         <v>1</v>
@@ -1141,7 +1141,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D28" s="5">
         <v>1</v>
@@ -1150,7 +1150,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D29" s="5">
         <v>1</v>
@@ -1212,7 +1212,12 @@
       <c r="E35" s="6"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D36" s="5"/>
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="5">
+        <v>1</v>
+      </c>
       <c r="E36" s="6"/>
     </row>
   </sheetData>

</xml_diff>